<commit_message>
updated attendance for CSC231
</commit_message>
<xml_diff>
--- a/attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
+++ b/attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -40,12 +40,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FF9999"/>
         <bgColor rgb="00FF9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF99"/>
-        <bgColor rgb="00FFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -67,13 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -439,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +476,16 @@
           <t>2025-09-09</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -520,6 +523,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -557,6 +570,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -594,6 +617,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -631,6 +664,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -663,9 +706,19 @@
           <t>0</t>
         </is>
       </c>
-      <c r="G6" s="2" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -705,6 +758,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -737,9 +800,19 @@
           <t>0</t>
         </is>
       </c>
-      <c r="G8" s="3" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>0.5</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -779,6 +852,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -816,6 +899,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -853,6 +946,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -890,6 +993,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -927,6 +1040,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -964,6 +1087,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1001,6 +1134,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1033,9 +1176,19 @@
           <t>0</t>
         </is>
       </c>
-      <c r="G16" s="2" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1075,6 +1228,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1112,6 +1275,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1149,6 +1322,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1186,6 +1369,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1223,6 +1416,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1255,10 +1458,18 @@
           <t>0</t>
         </is>
       </c>
-      <c r="G22" s="2" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>1</t>
         </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1297,6 +1508,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1334,6 +1555,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1371,6 +1602,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1408,6 +1649,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1440,8 +1691,20 @@
           <t>0</t>
         </is>
       </c>
-      <c r="G27" s="2" t="n">
-        <v>1</v>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1480,6 +1743,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1517,6 +1790,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1554,6 +1837,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1587,6 +1880,16 @@
         </is>
       </c>
       <c r="G31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
updated to fix the visualization
</commit_message>
<xml_diff>
--- a/attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
+++ b/attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
@@ -29,12 +29,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF99"/>
+        <bgColor rgb="00FFFF99"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -61,12 +67,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +493,11 @@
           <t>2025-09-18</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -533,6 +545,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -580,6 +597,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -627,6 +649,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -669,9 +696,14 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I5" s="2" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -721,6 +753,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -763,9 +800,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="I7" s="2" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -815,6 +857,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -862,6 +909,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -909,6 +961,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -956,6 +1013,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1003,6 +1065,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1050,6 +1117,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1097,6 +1169,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1144,6 +1221,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J15" s="2" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1191,6 +1273,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1238,6 +1325,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1285,6 +1377,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1332,6 +1429,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1379,6 +1481,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1426,6 +1533,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1468,8 +1580,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="I22" s="2" t="n">
-        <v>1</v>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1518,6 +1637,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1565,6 +1689,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1612,6 +1741,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1659,6 +1793,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1706,6 +1845,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1753,6 +1897,9 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J28" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1800,6 +1947,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1847,6 +1999,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1890,6 +2047,11 @@
         </is>
       </c>
       <c r="I31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
updated attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
</commit_message>
<xml_diff>
--- a/attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
+++ b/attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
@@ -38,14 +38,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF99"/>
-        <bgColor rgb="00FFFF99"/>
+        <fgColor rgb="00FF9999"/>
+        <bgColor rgb="00FF9999"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF9999"/>
-        <bgColor rgb="00FF9999"/>
+        <fgColor rgb="00FFFF99"/>
+        <bgColor rgb="00FFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,6 +498,11 @@
           <t>2025-09-23</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>2025-10-16</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -545,9 +550,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>0.5</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -602,6 +612,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -654,6 +669,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -706,6 +726,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -758,6 +783,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -810,6 +840,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -862,6 +897,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -914,6 +954,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -966,6 +1011,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1018,6 +1068,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1070,6 +1125,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1122,6 +1182,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1174,26 +1239,31 @@
           <t>0</t>
         </is>
       </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1034824</t>
+          <t>1035784</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Soliven</t>
+          <t>Gerken</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Madeline</t>
+          <t>Ryan</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1034824@wcupa.edu</t>
+          <t>1035784@wcupa.edu</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1208,12 +1278,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1221,31 +1291,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="J15" s="2" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1035784</t>
+          <t>1036641</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Gerken</t>
+          <t>Wesley</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Ryan</t>
+          <t>Benji</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1035784@wcupa.edu</t>
+          <t>1036641@wcupa.edu</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1260,7 +1335,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1274,6 +1349,11 @@
         </is>
       </c>
       <c r="J16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1282,22 +1362,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1036641</t>
+          <t>1040033</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Wesley</t>
+          <t>Pryszlak</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Benji</t>
+          <t>Zoya</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1036641@wcupa.edu</t>
+          <t>1040033@wcupa.edu</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1326,6 +1406,11 @@
         </is>
       </c>
       <c r="J17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1334,22 +1419,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1040033</t>
+          <t>1040690</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Pryszlak</t>
+          <t>Tapper</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Zoya</t>
+          <t>Darion</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1040033@wcupa.edu</t>
+          <t>1040690@wcupa.edu</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1359,7 +1444,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1378,6 +1463,11 @@
         </is>
       </c>
       <c r="J18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1386,22 +1476,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1040690</t>
+          <t>1042209</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Tapper</t>
+          <t>Amorose</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Darion</t>
+          <t>Jude</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1040690@wcupa.edu</t>
+          <t>1042209@wcupa.edu</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1411,7 +1501,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1430,6 +1520,11 @@
         </is>
       </c>
       <c r="J19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1438,22 +1533,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1042209</t>
+          <t>1045502</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Amorose</t>
+          <t>Dussintyl</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Jude</t>
+          <t>Shelby</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1042209@wcupa.edu</t>
+          <t>1045502@wcupa.edu</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1484,28 +1579,33 @@
       <c r="J20" t="inlineStr">
         <is>
           <t>0</t>
+        </is>
+      </c>
+      <c r="K20" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1045502</t>
+          <t>1047839</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Dussintyl</t>
+          <t>Zeltner</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Shelby</t>
+          <t>Jack</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1045502@wcupa.edu</t>
+          <t>1047839@wcupa.edu</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1520,7 +1620,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1530,10 +1630,15 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1542,22 +1647,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1047839</t>
+          <t>1050809</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Zeltner</t>
+          <t>McGurgan</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Jack</t>
+          <t>Shea</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1047839@wcupa.edu</t>
+          <t>1050809@wcupa.edu</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1572,7 +1677,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1582,10 +1687,15 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1594,27 +1704,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1050809</t>
+          <t>1052015</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>McGurgan</t>
+          <t>Monteith</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Shea</t>
+          <t>Amani</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1050809@wcupa.edu</t>
+          <t>1052015@wcupa.edu</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1638,6 +1748,11 @@
         </is>
       </c>
       <c r="J23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1646,27 +1761,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1052015</t>
+          <t>3000634</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Monteith</t>
+          <t>Brisita Perez</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Amani</t>
+          <t>Angeudy</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1052015@wcupa.edu</t>
+          <t>3000634@wcupa.edu</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1690,6 +1805,11 @@
         </is>
       </c>
       <c r="J24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1698,22 +1818,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>3000634</t>
+          <t>3018034</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Brisita Perez</t>
+          <t>Albarakati</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Angeudy</t>
+          <t>Nawaf</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3000634@wcupa.edu</t>
+          <t>3018034@wcupa.edu</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1742,6 +1862,11 @@
         </is>
       </c>
       <c r="J25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1750,22 +1875,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>3018034</t>
+          <t>3021493</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Albarakati</t>
+          <t>Schamis</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Nawaf</t>
+          <t>Levi</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3018034@wcupa.edu</t>
+          <t>3021493@wcupa.edu</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1780,7 +1905,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1795,29 +1920,34 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K26" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>3021493</t>
+          <t>3021762</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Schamis</t>
+          <t>Valades</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Levi</t>
+          <t>Cesar</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3021493@wcupa.edu</t>
+          <t>3021762@wcupa.edu</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1832,44 +1962,49 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J27" s="3" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3021762</t>
+          <t>3022161</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Valades</t>
+          <t>Nguyen</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Cesar</t>
+          <t>Huy</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3021762@wcupa.edu</t>
+          <t>3022161@wcupa.edu</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1897,29 +2032,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="J28" s="3" t="n">
-        <v>1</v>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3022161</t>
+          <t>3023729</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Nguyen</t>
+          <t>Fledderjohann</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Huy</t>
+          <t>Alec</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3022161@wcupa.edu</t>
+          <t>3023729@wcupa.edu</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1950,28 +2092,33 @@
       <c r="J29" t="inlineStr">
         <is>
           <t>0</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>0.5</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3023729</t>
+          <t>3023940</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Fledderjohann</t>
+          <t>Quinn</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Alec</t>
+          <t>Peter</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3023729@wcupa.edu</t>
+          <t>3023940@wcupa.edu</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2004,57 +2151,8 @@
           <t>0</t>
         </is>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>3023940</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Quinn</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Peter</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>3023940@wcupa.edu</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="K30" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and updated some files
</commit_message>
<xml_diff>
--- a/attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
+++ b/attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,6 +501,11 @@
           <t>2025-10-21</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>2025-10-28</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -563,6 +568,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -625,6 +635,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -687,6 +702,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -749,6 +769,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -806,7 +831,12 @@
           <t>1</t>
         </is>
       </c>
-      <c r="L6" s="2" t="inlineStr">
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M6" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -873,6 +903,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -935,6 +970,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -997,6 +1037,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1059,6 +1104,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1116,9 +1166,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L11" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1183,6 +1238,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1245,6 +1305,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1307,6 +1372,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1369,6 +1439,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1431,6 +1506,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1493,6 +1573,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1550,9 +1635,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L18" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1617,6 +1707,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1674,7 +1769,12 @@
           <t>1</t>
         </is>
       </c>
-      <c r="L20" s="2" t="inlineStr">
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M20" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1741,6 +1841,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1803,6 +1908,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M22" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1865,6 +1975,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1927,6 +2042,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1984,8 +2104,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L25" s="2" t="n">
-        <v>1</v>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -2049,6 +2176,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M26" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2111,6 +2243,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2173,6 +2310,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2230,6 +2372,11 @@
           <t>0.5</t>
         </is>
       </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2286,6 +2433,9 @@
         <is>
           <t>1</t>
         </is>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a PPT using beamer for CSC 231
</commit_message>
<xml_diff>
--- a/attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
+++ b/attendance/Fall 2025 CSC231-05 Computer Systems_GradesExport_2025-09-02-21-50.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -40,12 +40,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FF9999"/>
         <bgColor rgb="00FF9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF99"/>
-        <bgColor rgb="00FFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -67,13 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -439,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +511,11 @@
           <t>2025-11-11</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-20</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -590,6 +588,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -662,6 +665,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -734,6 +742,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -801,7 +814,12 @@
           <t>1</t>
         </is>
       </c>
-      <c r="N5" s="2" t="inlineStr">
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O5" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -873,9 +891,14 @@
           <t>1</t>
         </is>
       </c>
-      <c r="N6" s="3" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>0.5</t>
+        </is>
+      </c>
+      <c r="O6" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -950,6 +973,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1022,6 +1050,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1089,7 +1122,12 @@
           <t>0</t>
         </is>
       </c>
-      <c r="N9" s="2" t="inlineStr">
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O9" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1166,6 +1204,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1238,6 +1281,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1310,6 +1358,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O12" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1382,6 +1435,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O13" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1454,6 +1512,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1526,6 +1589,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1598,6 +1666,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O16" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1670,6 +1743,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1742,6 +1820,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1814,6 +1897,9 @@
           <t>0</t>
         </is>
       </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1881,7 +1967,7 @@
           <t>1</t>
         </is>
       </c>
-      <c r="N20" s="2" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -2591,8 +2677,10 @@
           <t>0</t>
         </is>
       </c>
-      <c r="N30" t="n">
-        <v>0</v>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>